<commit_message>
Change VARCHAR Length for Attributes in Employee Table and Improve Input Validation in Manage Page
</commit_message>
<xml_diff>
--- a/Bulk Users (Template).xlsx
+++ b/Bulk Users (Template).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvin\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABB71D1-9D81-48E3-8B1C-A351C49A8132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99647D48-F2DD-4701-BDBD-077502B20527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="865" yWindow="990" windowWidth="18105" windowHeight="8010" xr2:uid="{203CCFDA-507F-43E3-AA31-AF943FCECAF2}"/>
+    <workbookView xWindow="650" yWindow="3390" windowWidth="18105" windowHeight="8010" xr2:uid="{203CCFDA-507F-43E3-AA31-AF943FCECAF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -417,7 +417,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -464,9 +464,8 @@
     </row>
   </sheetData>
   <dataValidations count="9">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Email must be between 5 to 40 characters" sqref="F1:F1048576" xr:uid="{E1B420F4-BE0A-40D2-B591-0D1E24D62CC2}">
-      <formula1>5</formula1>
-      <formula2>40</formula2>
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Email maximum characters is 30 characters" sqref="F1:F1048576" xr:uid="{E1B420F4-BE0A-40D2-B591-0D1E24D62CC2}">
+      <formula1>31</formula1>
     </dataValidation>
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Department must be between 2 to 30 characters" sqref="G1:G1048576" xr:uid="{A0AC33B9-453E-4B83-9C50-D824EB17C3CE}">
       <formula1>2</formula1>
@@ -479,13 +478,13 @@
     <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Employee ID must be 5 characters only" sqref="A1:A1048576" xr:uid="{D130CE38-2D60-44C1-A9F7-651A5BC0377C}">
       <formula1>5</formula1>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Username must be between 5 to 20 characters" sqref="B1:B1048576" xr:uid="{BFC18C40-705E-470A-8C20-5175581C75C7}">
-      <formula1>5</formula1>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Username must be between 3 to 20 characters" sqref="B1:B1048576" xr:uid="{BFC18C40-705E-470A-8C20-5175581C75C7}">
+      <formula1>3</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Name must be between 5 to 50 characters" sqref="D1:D1048576" xr:uid="{AA0A53D8-9279-433C-BC23-D98665C8E724}">
-      <formula1>5</formula1>
-      <formula2>50</formula2>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Name must be between 3 to 37 characters" sqref="D1:D1048576" xr:uid="{AA0A53D8-9279-433C-BC23-D98665C8E724}">
+      <formula1>3</formula1>
+      <formula2>37</formula2>
     </dataValidation>
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Position must be between 5 to 30 characters" sqref="E1:E1048576" xr:uid="{02BF0367-D69F-4272-9A16-34AB58FA3C33}">
       <formula1>5</formula1>

</xml_diff>

<commit_message>
Improve UI Of The System and Bug Fixing
</commit_message>
<xml_diff>
--- a/Bulk Users (Template).xlsx
+++ b/Bulk Users (Template).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvin\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99647D48-F2DD-4701-BDBD-077502B20527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B592ED56-BB36-4D07-9A6C-9941318A7840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="650" yWindow="3390" windowWidth="18105" windowHeight="8010" xr2:uid="{203CCFDA-507F-43E3-AA31-AF943FCECAF2}"/>
+    <workbookView xWindow="1095" yWindow="2070" windowWidth="18105" windowHeight="8010" xr2:uid="{203CCFDA-507F-43E3-AA31-AF943FCECAF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -417,7 +417,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -486,8 +486,8 @@
       <formula1>3</formula1>
       <formula2>37</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Position must be between 5 to 30 characters" sqref="E1:E1048576" xr:uid="{02BF0367-D69F-4272-9A16-34AB58FA3C33}">
-      <formula1>5</formula1>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Position must be between 3 to 30 characters" sqref="E1:E1048576" xr:uid="{02BF0367-D69F-4272-9A16-34AB58FA3C33}">
+      <formula1>3</formula1>
       <formula2>30</formula2>
     </dataValidation>
     <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Password must be 32 characters" sqref="C1:C1048576" xr:uid="{417FBD70-FC12-4C8C-85BE-B0B7755EAD47}">

</xml_diff>